<commit_message>
changing initials for necro for calibration
</commit_message>
<xml_diff>
--- a/data_231_ms.xlsx
+++ b/data_231_ms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geenaildefonso/Projects/ParticleSwarmOptimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{748A404A-FEB0-EC47-9CCE-1CEF564A56F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29749A5A-1411-0143-813E-5A0E776D7A91}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{82B1D2C9-38A1-FF40-9776-93DC777C5E2D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{82B1D2C9-38A1-FF40-9776-93DC777C5E2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -465,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C27F9D-9374-BA42-B3B1-4BD0D081CF34}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>